<commit_message>
Test bmp hash codes
</commit_message>
<xml_diff>
--- a/Reports/test data 2.xlsx
+++ b/Reports/test data 2.xlsx
@@ -41,48 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>c_vector</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>name:</t>
-  </si>
-  <si>
-    <t>E_grey:</t>
-  </si>
-  <si>
-    <t>The</t>
-  </si>
-  <si>
-    <t>processing</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>seconds</t>
-  </si>
-  <si>
-    <t>Layer32x32_90.bmp</t>
-  </si>
-  <si>
-    <t>Layer32x32_180.bmp</t>
-  </si>
-  <si>
-    <t>4.106</t>
-  </si>
-  <si>
-    <t>Layer32x32_270.bmp</t>
-  </si>
-  <si>
-    <t>7.338</t>
   </si>
 </sst>
 </file>
@@ -3237,10 +3198,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C113:W146"/>
+  <dimension ref="C115:W139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="N139" sqref="N139:W139"/>
+      <selection activeCell="M123" sqref="M123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3253,1374 +3214,153 @@
     <col min="14" max="18" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="113" spans="3:23">
-      <c r="P113" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>2</v>
-      </c>
-      <c r="R113" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114" spans="3:23">
-      <c r="C114">
-        <v>267995</v>
-      </c>
-      <c r="D114">
-        <v>267995</v>
-      </c>
-      <c r="E114">
-        <v>267995</v>
-      </c>
-      <c r="F114">
-        <v>267995</v>
-      </c>
-      <c r="G114">
-        <v>267995</v>
-      </c>
-      <c r="H114">
-        <v>267995</v>
-      </c>
-      <c r="I114">
-        <v>267995</v>
-      </c>
-      <c r="J114">
-        <v>267995</v>
-      </c>
-      <c r="K114">
-        <v>267995</v>
-      </c>
-      <c r="L114">
-        <v>267995</v>
-      </c>
-      <c r="N114">
-        <v>243294</v>
-      </c>
-      <c r="O114">
-        <v>243294</v>
-      </c>
-      <c r="P114">
-        <v>243294</v>
-      </c>
-      <c r="Q114">
-        <v>243294</v>
-      </c>
-      <c r="R114">
-        <v>243294</v>
-      </c>
-      <c r="S114">
-        <v>243294</v>
-      </c>
-      <c r="T114">
-        <v>243294</v>
-      </c>
-      <c r="U114">
-        <v>243294</v>
-      </c>
-      <c r="V114">
-        <v>243294</v>
-      </c>
-      <c r="W114">
-        <v>243294</v>
-      </c>
-    </row>
     <row r="115" spans="3:23">
-      <c r="C115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="D115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="E115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="F115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="G115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="H115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="I115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="J115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="K115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="L115" s="1">
-        <v>451400</v>
-      </c>
-      <c r="N115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="O115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="P115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="Q115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="R115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="S115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="T115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="U115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="V115" s="1">
-        <v>325395</v>
-      </c>
-      <c r="W115" s="1">
-        <v>325395</v>
-      </c>
-    </row>
-    <row r="116" spans="3:23">
-      <c r="C116">
-        <v>393117</v>
-      </c>
-      <c r="D116">
-        <v>393117</v>
-      </c>
-      <c r="E116">
-        <v>393117</v>
-      </c>
-      <c r="F116">
-        <v>393117</v>
-      </c>
-      <c r="G116">
-        <v>393117</v>
-      </c>
-      <c r="H116">
-        <v>393117</v>
-      </c>
-      <c r="I116">
-        <v>393117</v>
-      </c>
-      <c r="J116">
-        <v>393117</v>
-      </c>
-      <c r="K116">
-        <v>393117</v>
-      </c>
-      <c r="L116">
-        <v>393117</v>
-      </c>
-      <c r="N116">
-        <v>255954</v>
-      </c>
-      <c r="O116">
-        <v>255954</v>
-      </c>
-      <c r="P116">
-        <v>255954</v>
-      </c>
-      <c r="Q116">
-        <v>255954</v>
-      </c>
-      <c r="R116">
-        <v>255954</v>
-      </c>
-      <c r="S116">
-        <v>255954</v>
-      </c>
-      <c r="T116">
-        <v>255954</v>
-      </c>
-      <c r="U116">
-        <v>255954</v>
-      </c>
-      <c r="V116">
-        <v>255954</v>
-      </c>
-      <c r="W116">
-        <v>255954</v>
-      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1"/>
+      <c r="R115" s="1"/>
+      <c r="S115" s="1"/>
+      <c r="T115" s="1"/>
+      <c r="U115" s="1"/>
+      <c r="V115" s="1"/>
+      <c r="W115" s="1"/>
     </row>
     <row r="117" spans="3:23">
-      <c r="C117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="D117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="E117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="F117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="G117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="H117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="I117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="J117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="K117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="L117" s="1">
-        <v>377705</v>
-      </c>
-      <c r="N117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="O117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="P117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="Q117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="R117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="S117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="T117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="U117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="V117" s="1">
-        <v>259359</v>
-      </c>
-      <c r="W117" s="1">
-        <v>259359</v>
-      </c>
-    </row>
-    <row r="118" spans="3:23">
-      <c r="C118">
-        <v>321599</v>
-      </c>
-      <c r="D118">
-        <v>321599</v>
-      </c>
-      <c r="E118">
-        <v>321599</v>
-      </c>
-      <c r="F118">
-        <v>321599</v>
-      </c>
-      <c r="G118">
-        <v>321599</v>
-      </c>
-      <c r="H118">
-        <v>321599</v>
-      </c>
-      <c r="I118">
-        <v>321599</v>
-      </c>
-      <c r="J118">
-        <v>321599</v>
-      </c>
-      <c r="K118">
-        <v>321599</v>
-      </c>
-      <c r="L118">
-        <v>321599</v>
-      </c>
-      <c r="N118">
-        <v>261079</v>
-      </c>
-      <c r="O118">
-        <v>261079</v>
-      </c>
-      <c r="P118">
-        <v>261079</v>
-      </c>
-      <c r="Q118">
-        <v>261079</v>
-      </c>
-      <c r="R118">
-        <v>261079</v>
-      </c>
-      <c r="S118">
-        <v>261079</v>
-      </c>
-      <c r="T118">
-        <v>261079</v>
-      </c>
-      <c r="U118">
-        <v>261079</v>
-      </c>
-      <c r="V118">
-        <v>261079</v>
-      </c>
-      <c r="W118">
-        <v>261079</v>
-      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="1"/>
+      <c r="R117" s="1"/>
+      <c r="S117" s="1"/>
+      <c r="T117" s="1"/>
+      <c r="U117" s="1"/>
+      <c r="V117" s="1"/>
+      <c r="W117" s="1"/>
     </row>
     <row r="119" spans="3:23">
-      <c r="C119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="D119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="E119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="F119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="G119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="H119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="I119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="J119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="K119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="L119" s="1">
-        <v>265703</v>
-      </c>
-      <c r="N119">
-        <v>277332</v>
-      </c>
-      <c r="O119">
-        <v>277332</v>
-      </c>
-      <c r="P119">
-        <v>277332</v>
-      </c>
-      <c r="Q119">
-        <v>277332</v>
-      </c>
-      <c r="R119">
-        <v>277332</v>
-      </c>
-      <c r="S119">
-        <v>277332</v>
-      </c>
-      <c r="T119">
-        <v>277332</v>
-      </c>
-      <c r="U119">
-        <v>277332</v>
-      </c>
-      <c r="V119">
-        <v>277332</v>
-      </c>
-      <c r="W119">
-        <v>277332</v>
-      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
     </row>
     <row r="120" spans="3:23">
-      <c r="C120">
-        <v>252586</v>
-      </c>
-      <c r="D120">
-        <v>252586</v>
-      </c>
-      <c r="E120">
-        <v>252586</v>
-      </c>
-      <c r="F120">
-        <v>252586</v>
-      </c>
-      <c r="G120">
-        <v>252586</v>
-      </c>
-      <c r="H120">
-        <v>252586</v>
-      </c>
-      <c r="I120">
-        <v>252586</v>
-      </c>
-      <c r="J120">
-        <v>252586</v>
-      </c>
-      <c r="K120">
-        <v>252586</v>
-      </c>
-      <c r="L120">
-        <v>252586</v>
-      </c>
-      <c r="N120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="O120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="P120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="Q120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="R120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="S120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="T120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="U120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="V120" s="1">
-        <v>296329</v>
-      </c>
-      <c r="W120" s="1">
-        <v>296329</v>
-      </c>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+      <c r="Q120" s="1"/>
+      <c r="R120" s="1"/>
+      <c r="S120" s="1"/>
+      <c r="T120" s="1"/>
+      <c r="U120" s="1"/>
+      <c r="V120" s="1"/>
+      <c r="W120" s="1"/>
     </row>
     <row r="121" spans="3:23">
-      <c r="C121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="D121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="E121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="F121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="G121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="H121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="I121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="J121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="K121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="L121" s="1">
-        <v>256442</v>
-      </c>
-      <c r="N121">
-        <v>322545</v>
-      </c>
-      <c r="O121">
-        <v>322545</v>
-      </c>
-      <c r="P121">
-        <v>322545</v>
-      </c>
-      <c r="Q121">
-        <v>322545</v>
-      </c>
-      <c r="R121">
-        <v>322545</v>
-      </c>
-      <c r="S121">
-        <v>322545</v>
-      </c>
-      <c r="T121">
-        <v>322545</v>
-      </c>
-      <c r="U121">
-        <v>322545</v>
-      </c>
-      <c r="V121">
-        <v>322545</v>
-      </c>
-      <c r="W121">
-        <v>322545</v>
-      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
     </row>
     <row r="122" spans="3:23">
-      <c r="C122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="D122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="E122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="F122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="G122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="H122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="I122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="J122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="K122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="L122" s="1">
-        <v>352542</v>
-      </c>
-      <c r="N122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="O122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="P122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="Q122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="R122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="S122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="T122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="U122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="V122" s="1">
-        <v>397912</v>
-      </c>
-      <c r="W122" s="1">
-        <v>397912</v>
-      </c>
-    </row>
-    <row r="123" spans="3:23">
-      <c r="C123">
-        <v>261366</v>
-      </c>
-      <c r="D123">
-        <v>261366</v>
-      </c>
-      <c r="E123">
-        <v>261366</v>
-      </c>
-      <c r="F123">
-        <v>261366</v>
-      </c>
-      <c r="G123">
-        <v>261366</v>
-      </c>
-      <c r="H123">
-        <v>261366</v>
-      </c>
-      <c r="I123">
-        <v>261366</v>
-      </c>
-      <c r="J123">
-        <v>261366</v>
-      </c>
-      <c r="K123">
-        <v>261366</v>
-      </c>
-      <c r="L123">
-        <v>261366</v>
-      </c>
-      <c r="N123">
-        <v>268224</v>
-      </c>
-      <c r="O123">
-        <v>268224</v>
-      </c>
-      <c r="P123">
-        <v>268224</v>
-      </c>
-      <c r="Q123">
-        <v>268224</v>
-      </c>
-      <c r="R123">
-        <v>268224</v>
-      </c>
-      <c r="S123">
-        <v>268224</v>
-      </c>
-      <c r="T123">
-        <v>268224</v>
-      </c>
-      <c r="U123">
-        <v>268224</v>
-      </c>
-      <c r="V123">
-        <v>268224</v>
-      </c>
-      <c r="W123">
-        <v>268224</v>
-      </c>
-    </row>
-    <row r="126" spans="3:23">
-      <c r="C126" t="s">
-        <v>3</v>
-      </c>
-      <c r="D126">
-        <v>98</v>
-      </c>
-      <c r="N126" t="s">
-        <v>3</v>
-      </c>
-      <c r="O126">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="127" spans="3:23">
-      <c r="C127" t="s">
-        <v>3</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="3:23">
-      <c r="C130" t="s">
-        <v>1</v>
-      </c>
-      <c r="D130" t="s">
-        <v>2</v>
-      </c>
-      <c r="E130" t="s">
-        <v>10</v>
-      </c>
-      <c r="O130" t="s">
-        <v>1</v>
-      </c>
-      <c r="P130" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q130" t="s">
-        <v>12</v>
-      </c>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+      <c r="Q122" s="1"/>
+      <c r="R122" s="1"/>
+      <c r="S122" s="1"/>
+      <c r="T122" s="1"/>
+      <c r="U122" s="1"/>
+      <c r="V122" s="1"/>
+      <c r="W122" s="1"/>
     </row>
     <row r="132" spans="3:23">
-      <c r="C132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="D132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="E132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="F132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="G132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="H132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="I132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="J132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="K132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="L132" s="1">
-        <v>252306</v>
-      </c>
-      <c r="N132">
-        <v>241804</v>
-      </c>
-      <c r="O132">
-        <v>241804</v>
-      </c>
-      <c r="P132">
-        <v>241804</v>
-      </c>
-      <c r="Q132">
-        <v>241804</v>
-      </c>
-      <c r="R132">
-        <v>241804</v>
-      </c>
-      <c r="S132">
-        <v>241804</v>
-      </c>
-      <c r="T132">
-        <v>241804</v>
-      </c>
-      <c r="U132">
-        <v>241804</v>
-      </c>
-      <c r="V132">
-        <v>241804</v>
-      </c>
-      <c r="W132">
-        <v>241804</v>
-      </c>
-    </row>
-    <row r="133" spans="3:23">
-      <c r="C133">
-        <v>367638</v>
-      </c>
-      <c r="D133">
-        <v>367638</v>
-      </c>
-      <c r="E133">
-        <v>367638</v>
-      </c>
-      <c r="F133">
-        <v>367638</v>
-      </c>
-      <c r="G133">
-        <v>367638</v>
-      </c>
-      <c r="H133">
-        <v>367638</v>
-      </c>
-      <c r="I133">
-        <v>367638</v>
-      </c>
-      <c r="J133">
-        <v>367638</v>
-      </c>
-      <c r="K133">
-        <v>367638</v>
-      </c>
-      <c r="L133">
-        <v>367638</v>
-      </c>
-      <c r="N133">
-        <v>323564</v>
-      </c>
-      <c r="O133">
-        <v>323564</v>
-      </c>
-      <c r="P133">
-        <v>323564</v>
-      </c>
-      <c r="Q133">
-        <v>323564</v>
-      </c>
-      <c r="R133">
-        <v>323564</v>
-      </c>
-      <c r="S133">
-        <v>323564</v>
-      </c>
-      <c r="T133">
-        <v>323564</v>
-      </c>
-      <c r="U133">
-        <v>323564</v>
-      </c>
-      <c r="V133">
-        <v>323564</v>
-      </c>
-      <c r="W133">
-        <v>323564</v>
-      </c>
-    </row>
-    <row r="134" spans="3:23">
-      <c r="C134">
-        <v>310074</v>
-      </c>
-      <c r="D134">
-        <v>310074</v>
-      </c>
-      <c r="E134">
-        <v>310074</v>
-      </c>
-      <c r="F134">
-        <v>310074</v>
-      </c>
-      <c r="G134">
-        <v>310074</v>
-      </c>
-      <c r="H134">
-        <v>310074</v>
-      </c>
-      <c r="I134">
-        <v>310074</v>
-      </c>
-      <c r="J134">
-        <v>310074</v>
-      </c>
-      <c r="K134">
-        <v>310074</v>
-      </c>
-      <c r="L134">
-        <v>310074</v>
-      </c>
-      <c r="N134">
-        <v>250949</v>
-      </c>
-      <c r="O134">
-        <v>250949</v>
-      </c>
-      <c r="P134">
-        <v>250949</v>
-      </c>
-      <c r="Q134">
-        <v>250949</v>
-      </c>
-      <c r="R134">
-        <v>250949</v>
-      </c>
-      <c r="S134">
-        <v>250949</v>
-      </c>
-      <c r="T134">
-        <v>250949</v>
-      </c>
-      <c r="U134">
-        <v>250949</v>
-      </c>
-      <c r="V134">
-        <v>250949</v>
-      </c>
-      <c r="W134">
-        <v>250949</v>
-      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
     </row>
     <row r="135" spans="3:23">
-      <c r="C135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="D135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="E135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="F135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="G135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="H135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="I135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="J135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="K135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="L135" s="1">
-        <v>318322</v>
-      </c>
-      <c r="N135">
-        <v>256134</v>
-      </c>
-      <c r="O135">
-        <v>256134</v>
-      </c>
-      <c r="P135">
-        <v>256134</v>
-      </c>
-      <c r="Q135">
-        <v>256134</v>
-      </c>
-      <c r="R135">
-        <v>256134</v>
-      </c>
-      <c r="S135">
-        <v>256134</v>
-      </c>
-      <c r="T135">
-        <v>256134</v>
-      </c>
-      <c r="U135">
-        <v>256134</v>
-      </c>
-      <c r="V135">
-        <v>256134</v>
-      </c>
-      <c r="W135">
-        <v>256134</v>
-      </c>
-    </row>
-    <row r="136" spans="3:23">
-      <c r="C136">
-        <v>316119</v>
-      </c>
-      <c r="D136">
-        <v>316119</v>
-      </c>
-      <c r="E136">
-        <v>316119</v>
-      </c>
-      <c r="F136">
-        <v>316119</v>
-      </c>
-      <c r="G136">
-        <v>316119</v>
-      </c>
-      <c r="H136">
-        <v>316119</v>
-      </c>
-      <c r="I136">
-        <v>316119</v>
-      </c>
-      <c r="J136">
-        <v>316119</v>
-      </c>
-      <c r="K136">
-        <v>316119</v>
-      </c>
-      <c r="L136">
-        <v>316119</v>
-      </c>
-      <c r="N136">
-        <v>271221</v>
-      </c>
-      <c r="O136">
-        <v>271221</v>
-      </c>
-      <c r="P136">
-        <v>271221</v>
-      </c>
-      <c r="Q136">
-        <v>271221</v>
-      </c>
-      <c r="R136">
-        <v>271221</v>
-      </c>
-      <c r="S136">
-        <v>271221</v>
-      </c>
-      <c r="T136">
-        <v>271221</v>
-      </c>
-      <c r="U136">
-        <v>271221</v>
-      </c>
-      <c r="V136">
-        <v>271221</v>
-      </c>
-      <c r="W136">
-        <v>271221</v>
-      </c>
-    </row>
-    <row r="137" spans="3:23">
-      <c r="C137">
-        <v>296674</v>
-      </c>
-      <c r="D137">
-        <v>296674</v>
-      </c>
-      <c r="E137">
-        <v>296674</v>
-      </c>
-      <c r="F137">
-        <v>296674</v>
-      </c>
-      <c r="G137">
-        <v>296674</v>
-      </c>
-      <c r="H137">
-        <v>296674</v>
-      </c>
-      <c r="I137">
-        <v>296674</v>
-      </c>
-      <c r="J137">
-        <v>296674</v>
-      </c>
-      <c r="K137">
-        <v>296674</v>
-      </c>
-      <c r="L137">
-        <v>296674</v>
-      </c>
-      <c r="N137">
-        <v>300066</v>
-      </c>
-      <c r="O137">
-        <v>300066</v>
-      </c>
-      <c r="P137">
-        <v>300066</v>
-      </c>
-      <c r="Q137">
-        <v>300066</v>
-      </c>
-      <c r="R137">
-        <v>300066</v>
-      </c>
-      <c r="S137">
-        <v>300066</v>
-      </c>
-      <c r="T137">
-        <v>300066</v>
-      </c>
-      <c r="U137">
-        <v>300066</v>
-      </c>
-      <c r="V137">
-        <v>300066</v>
-      </c>
-      <c r="W137">
-        <v>300066</v>
-      </c>
-    </row>
-    <row r="138" spans="3:23">
-      <c r="C138">
-        <v>272766</v>
-      </c>
-      <c r="D138">
-        <v>272766</v>
-      </c>
-      <c r="E138">
-        <v>272766</v>
-      </c>
-      <c r="F138">
-        <v>272766</v>
-      </c>
-      <c r="G138">
-        <v>272766</v>
-      </c>
-      <c r="H138">
-        <v>272766</v>
-      </c>
-      <c r="I138">
-        <v>272766</v>
-      </c>
-      <c r="J138">
-        <v>272766</v>
-      </c>
-      <c r="K138">
-        <v>272766</v>
-      </c>
-      <c r="L138">
-        <v>272766</v>
-      </c>
-      <c r="N138">
-        <v>341174</v>
-      </c>
-      <c r="O138">
-        <v>341174</v>
-      </c>
-      <c r="P138">
-        <v>341174</v>
-      </c>
-      <c r="Q138">
-        <v>341174</v>
-      </c>
-      <c r="R138">
-        <v>341174</v>
-      </c>
-      <c r="S138">
-        <v>341174</v>
-      </c>
-      <c r="T138">
-        <v>341174</v>
-      </c>
-      <c r="U138">
-        <v>341174</v>
-      </c>
-      <c r="V138">
-        <v>341174</v>
-      </c>
-      <c r="W138">
-        <v>341174</v>
-      </c>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
     </row>
     <row r="139" spans="3:23">
-      <c r="C139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="D139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="E139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="F139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="G139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="H139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="I139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="J139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="K139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="L139" s="1">
-        <v>260875</v>
-      </c>
-      <c r="N139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="O139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="P139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="Q139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="R139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="S139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="T139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="U139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="V139" s="1">
-        <v>381436</v>
-      </c>
-      <c r="W139" s="1">
-        <v>381436</v>
-      </c>
-    </row>
-    <row r="140" spans="3:23">
-      <c r="C140">
-        <v>348536</v>
-      </c>
-      <c r="D140">
-        <v>348536</v>
-      </c>
-      <c r="E140">
-        <v>348536</v>
-      </c>
-      <c r="F140">
-        <v>348536</v>
-      </c>
-      <c r="G140">
-        <v>348536</v>
-      </c>
-      <c r="H140">
-        <v>348536</v>
-      </c>
-      <c r="I140">
-        <v>348536</v>
-      </c>
-      <c r="J140">
-        <v>348536</v>
-      </c>
-      <c r="K140">
-        <v>348536</v>
-      </c>
-      <c r="L140">
-        <v>348536</v>
-      </c>
-      <c r="N140">
-        <v>461658</v>
-      </c>
-      <c r="O140">
-        <v>461658</v>
-      </c>
-      <c r="P140">
-        <v>461658</v>
-      </c>
-      <c r="Q140">
-        <v>461658</v>
-      </c>
-      <c r="R140">
-        <v>461658</v>
-      </c>
-      <c r="S140">
-        <v>461658</v>
-      </c>
-      <c r="T140">
-        <v>461658</v>
-      </c>
-      <c r="U140">
-        <v>461658</v>
-      </c>
-      <c r="V140">
-        <v>461658</v>
-      </c>
-      <c r="W140">
-        <v>461658</v>
-      </c>
-    </row>
-    <row r="141" spans="3:23">
-      <c r="C141">
-        <v>260350</v>
-      </c>
-      <c r="D141">
-        <v>260350</v>
-      </c>
-      <c r="E141">
-        <v>260350</v>
-      </c>
-      <c r="F141">
-        <v>260350</v>
-      </c>
-      <c r="G141">
-        <v>260350</v>
-      </c>
-      <c r="H141">
-        <v>260350</v>
-      </c>
-      <c r="I141">
-        <v>260350</v>
-      </c>
-      <c r="J141">
-        <v>260350</v>
-      </c>
-      <c r="K141">
-        <v>260350</v>
-      </c>
-      <c r="L141">
-        <v>260350</v>
-      </c>
-      <c r="N141">
-        <v>282194</v>
-      </c>
-      <c r="O141">
-        <v>282194</v>
-      </c>
-      <c r="P141">
-        <v>282194</v>
-      </c>
-      <c r="Q141">
-        <v>282194</v>
-      </c>
-      <c r="R141">
-        <v>282194</v>
-      </c>
-      <c r="S141">
-        <v>282194</v>
-      </c>
-      <c r="T141">
-        <v>282194</v>
-      </c>
-      <c r="U141">
-        <v>282194</v>
-      </c>
-      <c r="V141">
-        <v>282194</v>
-      </c>
-      <c r="W141">
-        <v>282194</v>
-      </c>
-    </row>
-    <row r="142" spans="3:23">
-      <c r="C142" t="s">
-        <v>3</v>
-      </c>
-      <c r="D142">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="143" spans="3:23">
-      <c r="C143" t="s">
-        <v>3</v>
-      </c>
-      <c r="D143">
-        <v>1</v>
-      </c>
-      <c r="N143" t="s">
-        <v>3</v>
-      </c>
-      <c r="O143">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="144" spans="3:23">
-      <c r="C144" t="s">
-        <v>4</v>
-      </c>
-      <c r="D144" t="s">
-        <v>5</v>
-      </c>
-      <c r="E144" t="s">
-        <v>6</v>
-      </c>
-      <c r="F144" t="s">
-        <v>7</v>
-      </c>
-      <c r="G144" t="s">
-        <v>11</v>
-      </c>
-      <c r="H144" t="s">
-        <v>8</v>
-      </c>
-      <c r="N144" t="s">
-        <v>3</v>
-      </c>
-      <c r="O144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="14:19">
-      <c r="N145" t="s">
-        <v>3</v>
-      </c>
-      <c r="O145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="14:19">
-      <c r="N146" t="s">
-        <v>4</v>
-      </c>
-      <c r="O146" t="s">
-        <v>5</v>
-      </c>
-      <c r="P146" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q146" t="s">
-        <v>7</v>
-      </c>
-      <c r="R146" t="s">
-        <v>13</v>
-      </c>
-      <c r="S146" t="s">
-        <v>8</v>
-      </c>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+      <c r="T139" s="1"/>
+      <c r="U139" s="1"/>
+      <c r="V139" s="1"/>
+      <c r="W139" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>